<commit_message>
Valores na reta final
</commit_message>
<xml_diff>
--- a/Preços.xlsx
+++ b/Preços.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellen\OneDrive\Área de Trabalho\Insper\eletromag\projeto\projeto-eletromag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/rafaeldbo_al_insper_edu_br/Documents/Programação/EletroMag-Workspace/projeto-eletromag/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43264BAC-5107-4EAE-BD77-3736D3CD127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{43264BAC-5107-4EAE-BD77-3736D3CD127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21E0D98-5467-44FC-89C1-6F798BB48F92}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" xr2:uid="{945A2026-313C-4BA3-9274-BDBF95F65ACA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{945A2026-313C-4BA3-9274-BDBF95F65ACA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela - prof" sheetId="1" r:id="rId1"/>
@@ -315,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,12 +330,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -404,7 +398,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -413,9 +407,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -423,6 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -755,11 +749,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B981AF-7EA4-4CC9-AF99-C5948D82E217}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="49.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
@@ -898,7 +892,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -1262,11 +1256,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228267F3-694F-42F4-B5E0-5281D0C062FF}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -1274,163 +1268,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>0.06</v>
       </c>
-      <c r="D2" s="5">
-        <f>B2*C2</f>
+      <c r="D2" s="4">
+        <f t="shared" ref="D2:D10" si="0">B2*C2</f>
         <v>0.06</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <f>SUM(D2:D10)</f>
         <v>148.41</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="11"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>28.16</v>
       </c>
-      <c r="D3" s="5">
-        <f>B3*C3</f>
+      <c r="D3" s="4">
+        <f t="shared" si="0"/>
         <v>28.16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1.8</v>
       </c>
-      <c r="D4" s="5">
-        <f>B4*C4</f>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.2</v>
       </c>
-      <c r="D5" s="5">
-        <f>B5*C5</f>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4">
         <v>6</v>
       </c>
-      <c r="D6" s="5">
-        <f>B6*C6</f>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="5">
-        <v>2</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
         <v>39.450000000000003</v>
       </c>
-      <c r="D7" s="5">
-        <f>B7*C7</f>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
         <v>78.900000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>0.23</v>
       </c>
-      <c r="D8" s="5">
-        <f>B8*C8</f>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
         <v>0.23</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="11">
+        <f>0.05*2</f>
         <v>0.1</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>134.6</v>
       </c>
-      <c r="D9" s="5">
-        <f>B9*C9</f>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
         <v>13.46</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>10</v>
       </c>
-      <c r="D10" s="5">
-        <f>B10*C10</f>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>

</xml_diff>